<commit_message>
Finished training new LSTM model
</commit_message>
<xml_diff>
--- a/LSTM and RNN examples/torques.xlsx
+++ b/LSTM and RNN examples/torques.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\malth\Documents\GitHub\Transparent-control-with-LSTM-and-FMG\LSTM and RNN examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A041020-B290-40B3-8A17-8FBA7E21F646}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5A21163-6AC8-4BBB-89ED-0DF0D82B8E52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1820" yWindow="1820" windowWidth="14400" windowHeight="7270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,11 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
-  <si>
-    <t>torque</t>
-  </si>
-</sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -388,7 +384,7 @@
   <dimension ref="A1:VV2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2175,9 +2171,7 @@
       </c>
     </row>
     <row r="2" spans="1:594" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="A2" s="1"/>
       <c r="B2">
         <v>-3.4012246876955032E-2</v>
       </c>

</xml_diff>